<commit_message>
Working on regression of data sets
</commit_message>
<xml_diff>
--- a/experimental_data/liver_volume/Thompson1965.xlsx
+++ b/experimental_data/liver_volume/Thompson1965.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Thompson1965 – Effect of age on liver function with particular reference to bromsulphalein extraction</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Body weight standard deviation [kg]</t>
+  </si>
+  <si>
+    <t>sample size</t>
   </si>
   <si>
     <t>status</t>
@@ -168,6 +171,7 @@
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -256,11 +260,11 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -356,7 +360,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -380,7 +384,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -509,11 +513,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="33591921"/>
-        <c:axId val="89634114"/>
+        <c:axId val="90750701"/>
+        <c:axId val="14350350"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33591921"/>
+        <c:axId val="90750701"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,7 +533,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>age groups [years]</a:t>
                 </a:r>
               </a:p>
@@ -547,11 +551,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="89634114"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="14350350"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89634114"/>
+        <c:axId val="14350350"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,7 +580,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>liver weight [kg]</a:t>
                 </a:r>
               </a:p>
@@ -594,8 +598,8 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="33591921"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="90750701"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -619,7 +623,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -643,7 +647,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -706,11 +710,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="15366"/>
-        <c:axId val="33494786"/>
+        <c:axId val="74980699"/>
+        <c:axId val="67658223"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="15366"/>
+        <c:axId val="74980699"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -726,7 +730,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>age groups [years]</a:t>
                 </a:r>
               </a:p>
@@ -744,11 +748,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="33494786"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="67658223"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33494786"/>
+        <c:axId val="67658223"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -773,7 +777,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
+                  <a:rPr b="1" sz="900"/>
                   <a:t>body weight [kg]</a:t>
                 </a:r>
               </a:p>
@@ -791,8 +795,8 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="15366"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="74980699"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -821,15 +825,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>25200</xdr:colOff>
+      <xdr:colOff>52200</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>92520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>177120</xdr:colOff>
+      <xdr:colOff>203760</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>28800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -844,8 +848,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="25200" y="3592440"/>
-          <a:ext cx="3416400" cy="3163680"/>
+          <a:off x="52200" y="3583440"/>
+          <a:ext cx="3416040" cy="3163320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -860,15 +864,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>347040</xdr:colOff>
+      <xdr:colOff>374040</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>498600</xdr:colOff>
+      <xdr:colOff>525240</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>47520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -883,8 +887,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="347040" y="6963120"/>
-          <a:ext cx="3416040" cy="3039120"/>
+          <a:off x="374040" y="6954120"/>
+          <a:ext cx="3415680" cy="3038760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -899,15 +903,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>449280</xdr:colOff>
+      <xdr:colOff>476280</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>200520</xdr:colOff>
+      <xdr:colOff>227160</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -915,8 +919,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3713760" y="3678480"/>
-        <a:ext cx="3200400" cy="2986920"/>
+        <a:off x="3740760" y="3669480"/>
+        <a:ext cx="3200040" cy="2986560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -929,15 +933,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>696240</xdr:colOff>
+      <xdr:colOff>723240</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:rowOff>44640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>584280</xdr:colOff>
+      <xdr:colOff>610920</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -945,8 +949,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3960720" y="6925320"/>
-        <a:ext cx="3337200" cy="2660400"/>
+        <a:off x="3987720" y="6916320"/>
+        <a:ext cx="3336840" cy="2660040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -966,8 +970,8 @@
   </sheetPr>
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11:L18"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="M18" activeCellId="0" pane="topLeft" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1008,7 +1012,7 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1016,7 +1020,7 @@
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1024,7 +1028,7 @@
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="4" t="n">
         <v>206</v>
       </c>
     </row>
@@ -1032,40 +1036,40 @@
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="57.45" outlineLevel="0" r="10" s="8">
       <c r="A10" s="7" t="s">
@@ -1104,341 +1108,367 @@
       <c r="L10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="0"/>
-      <c r="N10" s="0"/>
-      <c r="O10" s="0"/>
-      <c r="P10" s="0"/>
-      <c r="Q10" s="0"/>
-      <c r="R10" s="0"/>
-      <c r="S10" s="0"/>
-      <c r="T10" s="0"/>
-      <c r="U10" s="0"/>
-      <c r="V10" s="0"/>
-      <c r="W10" s="0"/>
-      <c r="X10" s="0"/>
+      <c r="M10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="11">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="9" t="s">
+      <c r="E12" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F12" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="K11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="4" t="n">
         <v>1.9750267</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="4" t="n">
         <v>2.4011467</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="4" t="n">
         <f aca="false">H12-G12</f>
         <v>0.42612</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J12" s="4" t="n">
         <v>71.62693</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="4" t="n">
         <v>92.30764</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12" s="4" t="n">
         <f aca="false">K12-J12</f>
         <v>20.68071</v>
       </c>
+      <c r="M12" s="0" t="n">
+        <v>25</v>
+      </c>
       <c r="P12" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
-      <c r="A13" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="0" t="s">
+      <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="B13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="C13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="4" t="n">
         <v>1.9051987</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="4" t="n">
         <v>2.3515499</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="4" t="n">
         <f aca="false">H13-G13</f>
         <v>0.4463512</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="J13" s="4" t="n">
         <v>58.54801</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="4" t="n">
         <v>70.728714</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13" s="4" t="n">
         <f aca="false">K13-J13</f>
         <v>12.180704</v>
       </c>
+      <c r="M13" s="0" t="n">
+        <v>25</v>
+      </c>
       <c r="P13" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="A14" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="A14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="C14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="4" t="n">
         <v>45</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="4" t="n">
         <v>1.8859974</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="4" t="n">
         <v>2.406763</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="4" t="n">
         <f aca="false">H14-G14</f>
         <v>0.5207656</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="J14" s="4" t="n">
         <v>63.881454</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="4" t="n">
         <v>81.72929</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="L14" s="4" t="n">
         <f aca="false">K14-J14</f>
         <v>17.847836</v>
       </c>
+      <c r="M14" s="0" t="n">
+        <v>25</v>
+      </c>
       <c r="P14" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
-      <c r="A15" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="B15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="C15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="4" t="n">
         <v>55</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="4" t="n">
         <v>1.762064</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="4" t="n">
         <v>2.174638</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="4" t="n">
         <f aca="false">H15-G15</f>
         <v>0.412574</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J15" s="4" t="n">
         <v>68.93297</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="4" t="n">
         <v>89.04778</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15" s="4" t="n">
         <f aca="false">K15-J15</f>
         <v>20.11481</v>
       </c>
+      <c r="M15" s="0" t="n">
+        <v>43</v>
+      </c>
       <c r="P15" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
-      <c r="A16" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="0" t="s">
+      <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="C16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="4" t="n">
         <v>65</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="4" t="n">
         <v>70</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="4" t="n">
         <v>1.6684676</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="4" t="n">
         <v>2.1791275</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="4" t="n">
         <f aca="false">H16-G16</f>
         <v>0.5106599</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="J16" s="4" t="n">
         <v>62.370358</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="K16" s="4" t="n">
         <v>79.36764</v>
       </c>
-      <c r="L16" s="0" t="n">
+      <c r="L16" s="4" t="n">
         <f aca="false">K16-J16</f>
         <v>16.997282</v>
       </c>
+      <c r="M16" s="0" t="n">
+        <v>64</v>
+      </c>
       <c r="P16" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
-      <c r="A17" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="0" t="s">
+      <c r="A17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="B17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="C17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="4" t="n">
         <v>75</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="4" t="n">
         <v>70</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="4" t="n">
         <v>1.442989</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="4" t="n">
         <v>1.6222136</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="4" t="n">
         <f aca="false">H17-G17</f>
         <v>0.1792246</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="J17" s="4" t="n">
         <v>58.07405</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="K17" s="4" t="n">
         <v>72.80503</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="L17" s="4" t="n">
         <f aca="false">K17-J17</f>
         <v>14.73098</v>
       </c>
+      <c r="M17" s="0" t="n">
+        <v>53</v>
+      </c>
       <c r="P17" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
-      <c r="A18" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="0" t="s">
+      <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="B18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="C18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="4" t="n">
         <v>85</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="4" t="n">
         <v>1.2073851</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="4" t="n">
         <v>1.3697016</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="I18" s="4" t="n">
         <f aca="false">H18-G18</f>
         <v>0.1623165</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="J18" s="4" t="n">
         <v>48.395267</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="K18" s="4" t="n">
         <v>61.991734</v>
       </c>
-      <c r="L18" s="0" t="n">
+      <c r="L18" s="4" t="n">
         <f aca="false">K18-J18</f>
         <v>13.596467</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>21</v>
       </c>
       <c r="P18" s="10"/>
     </row>

</xml_diff>